<commit_message>
Update JOCKEY CLUB_Orç. Páscoa 2023 - Jockey.xlsx
</commit_message>
<xml_diff>
--- a/orcamentos/JOCKEY CLUB_Orç. Páscoa 2023 - Jockey.xlsx
+++ b/orcamentos/JOCKEY CLUB_Orç. Páscoa 2023 - Jockey.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\GitHub\myxlsm\orcamentos\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F43B86EE-CBC2-43FC-9C35-8AC213431E4F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D739C618-2EDB-40B9-ACAD-71EC5AE2B9A7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" activeTab="4" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -17,8 +17,9 @@
     <sheet name="paraFilter" sheetId="6" r:id="rId2"/>
     <sheet name="resultado" sheetId="5" r:id="rId3"/>
     <sheet name="cenarios" sheetId="4" r:id="rId4"/>
-    <sheet name="Cenário Feliz Páscoa - Geral" sheetId="8" r:id="rId5"/>
-    <sheet name="Entrada Principal" sheetId="7" r:id="rId6"/>
+    <sheet name="Toca do Coelho - Ceário Geral" sheetId="9" r:id="rId5"/>
+    <sheet name="Cenário Feliz Páscoa - Geral" sheetId="8" r:id="rId6"/>
+    <sheet name="Entrada Principal" sheetId="7" r:id="rId7"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -39,7 +40,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="243" uniqueCount="160">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="298" uniqueCount="185">
   <si>
     <t>id</t>
   </si>
@@ -519,6 +520,81 @@
   </si>
   <si>
     <t>Cogumelo com portinha pintada, tridimensional, pintura colorida com predominância das cores vermelho e verde, medindo entre: mínimo: 0,23m de altura x 0,31m de largura x 0,38m de profundidade / máximo: 0,33m de altura x 0,41m de largura x 0,41m de profundidade, confeccionado em fibra de  vidro com acabamento liso e pintura com esmalte sintético e verniz automotivo brilhante.</t>
+  </si>
+  <si>
+    <t>FG35</t>
+  </si>
+  <si>
+    <t>0,52</t>
+  </si>
+  <si>
+    <t>0,46</t>
+  </si>
+  <si>
+    <t>Cogumelo, tridimensional,  medindo aproximadamente 0,50m de altura x 0,52m de largura x 0,46m de profundidade, confeccionado em fibra de vidro com acabamento liso e pintura com esmalte sintético e verniz automotivo brilhante.</t>
+  </si>
+  <si>
+    <t>Cogumelo com portinha pintada, tridimensional, pintura colorida com predominância das cores vermelho e verde, medindo entre: mínimo: 0,45m de altura x 0,47m de largura x 0,41m de profundidade / máximo: 0,55m de altura x 0,57m de largura x 0,51m de profundidade, confeccionado em fibra de  vidro com acabamento liso e pintura com esmalte sintético e verniz automotivo brilhante.</t>
+  </si>
+  <si>
+    <t>PFG03BGAZ</t>
+  </si>
+  <si>
+    <t>Ovo de páscoa tridimensional, pintado na cor azul com adesivo em forma de bolinhas brancas, medindo 0,75m de altura por 0,52m de diâmetro, produzido em fibra de vidro com acabamento liso e pintura com esmalte sintético e verniz automotivo brilhante.</t>
+  </si>
+  <si>
+    <t>Ovo de páscoa na cor azul com bolinhas brancas tridimensional alusivo a decoração de páscoa, com dimensões proporcionais entre mínimo: 0,70m altura x 0,47m diâmetro / máximo: 0,80m altura x 0,57m diâmetro. Produzido em fibra de  vidro com acabamento liso e pintura com esmalte sintético e verniz automotivo brilhante.</t>
+  </si>
+  <si>
+    <t>PFG03BMRS</t>
+  </si>
+  <si>
+    <t>Ovo de páscoa tridimensional, pintado na cor rosa com adesivo em forma de bolinhas brancas, medindo 0,50m de altura por 0,34m de diâmetro, produzido em fibra de vidro com acabamento liso e pintura com esmalte sintético e verniz automotivo brilhante.</t>
+  </si>
+  <si>
+    <t>Ovo de páscoa na cor rosa com bolinhas brancas tridimensional alusivo a decoração de páscoa, com dimensões proporcionais entre mínimo: 0,45m altura x 0,29m diâmetro / máximo: 0,55m altura x 0,39m diâmetro. Produzido em fibra de  vidro com acabamento liso e pintura com esmalte sintético e verniz automotivo brilhante.</t>
+  </si>
+  <si>
+    <t>FG133C</t>
+  </si>
+  <si>
+    <t>2,35</t>
+  </si>
+  <si>
+    <t>3,5</t>
+  </si>
+  <si>
+    <t>1,82</t>
+  </si>
+  <si>
+    <t>Balanço com três bancos em formato de bola,  produzido em fibra de vidro e estrutura metálica, com pintura automotiva linha candy.</t>
+  </si>
+  <si>
+    <t>Toca do Coelho - Ceário Geral</t>
+  </si>
+  <si>
+    <t>PFG17</t>
+  </si>
+  <si>
+    <t>3,2</t>
+  </si>
+  <si>
+    <t>3,05</t>
+  </si>
+  <si>
+    <t>Casa Cogumelo de chocolate c/ confetes, produzida em fibra de vidro</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Cogumelo gigante de chocolate com confetes, medindo aproximadamente 3,20m de altura x 3,05m de comprimento x 3,05m de largura confeccionado em fibra de vidro com acabamento liso e pintura com esmalte sintético e verniz automotivo brilhante. </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Casa em formato de cogumelo gigante, com pintura marrom imitando chocolate e aplicação de adesivos impressos imitando confetes. Produto tridimensional alusivo a decoração de páscoa. Produzida em fibra de  vidro com acabamento liso e pintura em esmalte sintético e verniz automotivo brilhante. Medidas entre: mínimo: 3,15m altura x 3,00m diâmetro / máximo: 3,25m altura x 3,15m diâmetro. </t>
+  </si>
+  <si>
+    <t>PMOBP02RF</t>
+  </si>
+  <si>
+    <t>Poste com floreiras confeccionados em fibra de vidro com pintura automotiva na cor rosa e detalhes em verde para o poste e caramelo para as floreiras, detalhes em estrutura de arabescos e luminária translúcida. OBS.: flores não inclusas.</t>
   </si>
 </sst>
 </file>
@@ -1006,7 +1082,7 @@
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <sheetPr codeName="Planilha4"/>
-  <dimension ref="A1:B3"/>
+  <dimension ref="A1:B4"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="G17" sqref="G17"/>
@@ -1042,14 +1118,22 @@
         <v>60</v>
       </c>
     </row>
+    <row r="4" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A4">
+        <v>4</v>
+      </c>
+      <c r="B4" t="s">
+        <v>176</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1954A817-8B83-4AEA-A467-593A05541A84}">
-  <dimension ref="A1:M26"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{76189D25-7218-4820-80E4-7C79DCBAE09C}">
+  <dimension ref="A1:M4"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
@@ -1101,35 +1185,35 @@
         <v>1</v>
       </c>
       <c r="B2" t="s">
-        <v>61</v>
+        <v>177</v>
       </c>
       <c r="C2">
         <v>1</v>
       </c>
-      <c r="D2">
-        <v>3</v>
-      </c>
-      <c r="E2">
-        <v>4</v>
-      </c>
-      <c r="F2">
-        <v>4</v>
+      <c r="D2" t="s">
+        <v>178</v>
+      </c>
+      <c r="E2" t="s">
+        <v>179</v>
+      </c>
+      <c r="F2" t="s">
+        <v>179</v>
       </c>
       <c r="H2" s="2">
-        <v>47324.537900000003</v>
+        <v>26771.9535</v>
       </c>
       <c r="J2" t="s">
-        <v>62</v>
+        <v>180</v>
       </c>
       <c r="K2" t="s">
-        <v>63</v>
+        <v>181</v>
       </c>
       <c r="L2" t="s">
-        <v>64</v>
+        <v>182</v>
       </c>
       <c r="M2">
-        <f t="shared" ref="M2:M7" si="0">C2*H2</f>
-        <v>47324.537900000003</v>
+        <f>C2*H2</f>
+        <v>26771.9535</v>
       </c>
     </row>
     <row r="3" spans="1:13" x14ac:dyDescent="0.3">
@@ -1137,32 +1221,17 @@
         <v>2</v>
       </c>
       <c r="B3" t="s">
-        <v>65</v>
+        <v>183</v>
       </c>
       <c r="C3">
-        <v>1</v>
-      </c>
-      <c r="D3" t="s">
-        <v>29</v>
-      </c>
-      <c r="E3" t="s">
-        <v>29</v>
-      </c>
-      <c r="F3" t="s">
-        <v>29</v>
-      </c>
-      <c r="G3">
+        <v>2</v>
+      </c>
+      <c r="H3" s="2">
         <v>0</v>
       </c>
-      <c r="H3" s="2">
-        <v>3843.9929000000002</v>
-      </c>
-      <c r="J3" t="s">
-        <v>66</v>
-      </c>
       <c r="M3">
-        <f t="shared" si="0"/>
-        <v>3843.9929000000002</v>
+        <f>C3*H3</f>
+        <v>0</v>
       </c>
     </row>
     <row r="4" spans="1:13" x14ac:dyDescent="0.3">
@@ -1170,746 +1239,32 @@
         <v>3</v>
       </c>
       <c r="B4" t="s">
-        <v>67</v>
+        <v>183</v>
       </c>
       <c r="C4">
         <v>1</v>
       </c>
       <c r="D4" t="s">
-        <v>68</v>
-      </c>
-      <c r="E4" t="s">
-        <v>69</v>
+        <v>50</v>
+      </c>
+      <c r="E4">
+        <v>1</v>
       </c>
       <c r="F4" t="s">
-        <v>70</v>
+        <v>51</v>
+      </c>
+      <c r="G4">
+        <v>0</v>
       </c>
       <c r="H4" s="2">
-        <v>3781.2494999999999</v>
+        <v>3673.2150000000001</v>
       </c>
       <c r="J4" t="s">
-        <v>71</v>
-      </c>
-      <c r="K4" t="s">
-        <v>72</v>
-      </c>
-      <c r="L4" t="s">
-        <v>73</v>
+        <v>184</v>
       </c>
       <c r="M4">
-        <f t="shared" si="0"/>
-        <v>3781.2494999999999</v>
-      </c>
-    </row>
-    <row r="5" spans="1:13" x14ac:dyDescent="0.3">
-      <c r="A5">
-        <v>4</v>
-      </c>
-      <c r="B5" t="s">
-        <v>74</v>
-      </c>
-      <c r="C5">
-        <v>1</v>
-      </c>
-      <c r="D5" t="s">
-        <v>75</v>
-      </c>
-      <c r="E5" t="s">
-        <v>76</v>
-      </c>
-      <c r="F5" t="s">
-        <v>77</v>
-      </c>
-      <c r="H5" s="2">
-        <v>5282.1998000000003</v>
-      </c>
-      <c r="J5" t="s">
-        <v>78</v>
-      </c>
-      <c r="M5">
-        <f t="shared" si="0"/>
-        <v>5282.1998000000003</v>
-      </c>
-    </row>
-    <row r="6" spans="1:13" x14ac:dyDescent="0.3">
-      <c r="A6">
-        <v>5</v>
-      </c>
-      <c r="B6" t="s">
-        <v>79</v>
-      </c>
-      <c r="C6">
-        <v>1</v>
-      </c>
-      <c r="D6" t="s">
-        <v>80</v>
-      </c>
-      <c r="H6" s="2">
-        <v>2818.92</v>
-      </c>
-      <c r="J6" t="s">
-        <v>81</v>
-      </c>
-      <c r="K6" t="s">
-        <v>82</v>
-      </c>
-      <c r="L6" t="s">
-        <v>83</v>
-      </c>
-      <c r="M6">
-        <f t="shared" si="0"/>
-        <v>2818.92</v>
-      </c>
-    </row>
-    <row r="7" spans="1:13" x14ac:dyDescent="0.3">
-      <c r="A7">
-        <v>6</v>
-      </c>
-      <c r="B7" t="s">
-        <v>84</v>
-      </c>
-      <c r="C7">
-        <v>1</v>
-      </c>
-      <c r="D7" t="s">
-        <v>85</v>
-      </c>
-      <c r="H7" s="2">
-        <v>951.5376</v>
-      </c>
-      <c r="J7" t="s">
-        <v>86</v>
-      </c>
-      <c r="K7" t="s">
-        <v>87</v>
-      </c>
-      <c r="L7" t="s">
-        <v>88</v>
-      </c>
-      <c r="M7">
-        <f t="shared" si="0"/>
-        <v>951.5376</v>
-      </c>
-    </row>
-    <row r="8" spans="1:13" x14ac:dyDescent="0.3">
-      <c r="A8">
-        <v>7</v>
-      </c>
-      <c r="B8" t="s">
-        <v>89</v>
-      </c>
-      <c r="C8">
-        <v>1</v>
-      </c>
-      <c r="D8" t="s">
-        <v>90</v>
-      </c>
-      <c r="E8" t="s">
-        <v>91</v>
-      </c>
-      <c r="F8" t="s">
-        <v>91</v>
-      </c>
-      <c r="H8" s="2">
-        <v>407.93220000000002</v>
-      </c>
-      <c r="J8" t="s">
-        <v>92</v>
-      </c>
-      <c r="K8" t="s">
-        <v>93</v>
-      </c>
-      <c r="L8" t="s">
-        <v>94</v>
-      </c>
-      <c r="M8">
-        <f t="shared" ref="M8:M13" si="1">C8*H8</f>
-        <v>407.93220000000002</v>
-      </c>
-    </row>
-    <row r="9" spans="1:13" x14ac:dyDescent="0.3">
-      <c r="A9">
-        <v>8</v>
-      </c>
-      <c r="B9" t="s">
-        <v>95</v>
-      </c>
-      <c r="C9">
-        <v>1</v>
-      </c>
-      <c r="D9" t="s">
-        <v>96</v>
-      </c>
-      <c r="E9" t="s">
-        <v>77</v>
-      </c>
-      <c r="F9">
-        <v>6</v>
-      </c>
-      <c r="H9" s="2">
-        <v>70702.5</v>
-      </c>
-      <c r="J9" t="s">
-        <v>97</v>
-      </c>
-      <c r="K9" t="s">
-        <v>98</v>
-      </c>
-      <c r="L9" t="s">
-        <v>99</v>
-      </c>
-      <c r="M9">
-        <f t="shared" si="1"/>
-        <v>70702.5</v>
-      </c>
-    </row>
-    <row r="10" spans="1:13" x14ac:dyDescent="0.3">
-      <c r="A10">
-        <v>9</v>
-      </c>
-      <c r="B10" t="s">
-        <v>100</v>
-      </c>
-      <c r="C10">
-        <v>1</v>
-      </c>
-      <c r="D10" t="s">
-        <v>101</v>
-      </c>
-      <c r="E10" t="s">
-        <v>75</v>
-      </c>
-      <c r="F10" t="s">
-        <v>75</v>
-      </c>
-      <c r="H10" s="2">
-        <v>4370.9639999999999</v>
-      </c>
-      <c r="J10" t="s">
-        <v>102</v>
-      </c>
-      <c r="K10" t="s">
-        <v>103</v>
-      </c>
-      <c r="L10" t="s">
-        <v>104</v>
-      </c>
-      <c r="M10">
-        <f t="shared" si="1"/>
-        <v>4370.9639999999999</v>
-      </c>
-    </row>
-    <row r="11" spans="1:13" x14ac:dyDescent="0.3">
-      <c r="A11">
-        <v>10</v>
-      </c>
-      <c r="B11" t="s">
-        <v>105</v>
-      </c>
-      <c r="C11">
-        <v>1</v>
-      </c>
-      <c r="D11" t="s">
-        <v>29</v>
-      </c>
-      <c r="E11" t="s">
-        <v>106</v>
-      </c>
-      <c r="F11" t="s">
-        <v>107</v>
-      </c>
-      <c r="H11" s="2">
-        <v>25450</v>
-      </c>
-      <c r="J11" t="s">
-        <v>108</v>
-      </c>
-      <c r="L11" t="s">
-        <v>109</v>
-      </c>
-      <c r="M11">
-        <f t="shared" si="1"/>
-        <v>25450</v>
-      </c>
-    </row>
-    <row r="12" spans="1:13" x14ac:dyDescent="0.3">
-      <c r="A12">
-        <v>11</v>
-      </c>
-      <c r="B12" t="s">
-        <v>110</v>
-      </c>
-      <c r="C12">
-        <v>1</v>
-      </c>
-      <c r="D12" t="s">
-        <v>111</v>
-      </c>
-      <c r="E12" t="s">
-        <v>76</v>
-      </c>
-      <c r="F12" t="s">
-        <v>76</v>
-      </c>
-      <c r="H12" s="2">
-        <v>6624.7093000000004</v>
-      </c>
-      <c r="J12" t="s">
-        <v>112</v>
-      </c>
-      <c r="K12" t="s">
-        <v>113</v>
-      </c>
-      <c r="L12" t="s">
-        <v>114</v>
-      </c>
-      <c r="M12">
-        <f t="shared" si="1"/>
-        <v>6624.7093000000004</v>
-      </c>
-    </row>
-    <row r="13" spans="1:13" x14ac:dyDescent="0.3">
-      <c r="A13">
-        <v>12</v>
-      </c>
-      <c r="B13" t="s">
-        <v>115</v>
-      </c>
-      <c r="C13">
-        <v>1</v>
-      </c>
-      <c r="D13" t="s">
-        <v>116</v>
-      </c>
-      <c r="E13" t="s">
-        <v>117</v>
-      </c>
-      <c r="F13" t="s">
-        <v>117</v>
-      </c>
-      <c r="H13" s="2">
-        <v>5262.66</v>
-      </c>
-      <c r="J13" t="s">
-        <v>118</v>
-      </c>
-      <c r="M13">
-        <f t="shared" si="1"/>
-        <v>5262.66</v>
-      </c>
-    </row>
-    <row r="14" spans="1:13" x14ac:dyDescent="0.3">
-      <c r="A14">
-        <v>13</v>
-      </c>
-      <c r="B14" t="s">
-        <v>122</v>
-      </c>
-      <c r="C14">
-        <v>1</v>
-      </c>
-      <c r="D14" t="s">
-        <v>35</v>
-      </c>
-      <c r="E14" t="s">
-        <v>75</v>
-      </c>
-      <c r="F14" t="s">
-        <v>75</v>
-      </c>
-      <c r="H14" s="2">
-        <v>2985.2159999999999</v>
-      </c>
-      <c r="J14" t="s">
-        <v>123</v>
-      </c>
-      <c r="M14">
-        <f t="shared" ref="M14:M19" si="2">C14*H14</f>
-        <v>2985.2159999999999</v>
-      </c>
-    </row>
-    <row r="15" spans="1:13" x14ac:dyDescent="0.3">
-      <c r="A15">
-        <v>14</v>
-      </c>
-      <c r="B15" t="s">
-        <v>124</v>
-      </c>
-      <c r="C15">
-        <v>1</v>
-      </c>
-      <c r="D15" t="s">
-        <v>90</v>
-      </c>
-      <c r="E15" t="s">
-        <v>125</v>
-      </c>
-      <c r="F15" t="s">
-        <v>125</v>
-      </c>
-      <c r="H15" s="2">
-        <v>1571.7</v>
-      </c>
-      <c r="J15" t="s">
-        <v>126</v>
-      </c>
-      <c r="M15">
-        <f t="shared" si="2"/>
-        <v>1571.7</v>
-      </c>
-    </row>
-    <row r="16" spans="1:13" x14ac:dyDescent="0.3">
-      <c r="A16">
-        <v>15</v>
-      </c>
-      <c r="B16" t="s">
-        <v>127</v>
-      </c>
-      <c r="C16">
-        <v>1</v>
-      </c>
-      <c r="D16" t="s">
-        <v>128</v>
-      </c>
-      <c r="E16" t="s">
-        <v>111</v>
-      </c>
-      <c r="F16" t="s">
-        <v>111</v>
-      </c>
-      <c r="H16" s="2">
-        <v>9873</v>
-      </c>
-      <c r="J16" t="s">
-        <v>129</v>
-      </c>
-      <c r="K16" t="s">
-        <v>130</v>
-      </c>
-      <c r="L16" t="s">
-        <v>131</v>
-      </c>
-      <c r="M16">
-        <f t="shared" si="2"/>
-        <v>9873</v>
-      </c>
-    </row>
-    <row r="17" spans="1:13" x14ac:dyDescent="0.3">
-      <c r="A17">
-        <v>16</v>
-      </c>
-      <c r="B17" t="s">
-        <v>132</v>
-      </c>
-      <c r="D17">
-        <v>15</v>
-      </c>
-      <c r="E17" t="s">
-        <v>133</v>
-      </c>
-      <c r="F17" t="s">
-        <v>134</v>
-      </c>
-      <c r="H17" s="2">
-        <v>0</v>
-      </c>
-      <c r="J17" t="s">
-        <v>135</v>
-      </c>
-      <c r="K17" t="s">
-        <v>136</v>
-      </c>
-      <c r="L17" t="s">
-        <v>137</v>
-      </c>
-      <c r="M17">
-        <f t="shared" si="2"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="18" spans="1:13" x14ac:dyDescent="0.3">
-      <c r="A18">
-        <v>17</v>
-      </c>
-      <c r="B18" t="s">
-        <v>138</v>
-      </c>
-      <c r="C18">
-        <v>1</v>
-      </c>
-      <c r="H18" s="2">
-        <v>0</v>
-      </c>
-      <c r="J18" t="s">
-        <v>139</v>
-      </c>
-      <c r="M18">
-        <f t="shared" si="2"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="19" spans="1:13" x14ac:dyDescent="0.3">
-      <c r="A19">
-        <v>18</v>
-      </c>
-      <c r="B19" t="s">
-        <v>140</v>
-      </c>
-      <c r="C19">
-        <v>1</v>
-      </c>
-      <c r="D19">
-        <v>15</v>
-      </c>
-      <c r="E19" t="s">
-        <v>133</v>
-      </c>
-      <c r="F19" t="s">
-        <v>134</v>
-      </c>
-      <c r="H19" s="2">
-        <v>0</v>
-      </c>
-      <c r="J19" t="s">
-        <v>141</v>
-      </c>
-      <c r="K19" t="s">
-        <v>142</v>
-      </c>
-      <c r="L19" t="s">
-        <v>143</v>
-      </c>
-      <c r="M19">
-        <f t="shared" si="2"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="20" spans="1:13" x14ac:dyDescent="0.3">
-      <c r="A20">
-        <v>19</v>
-      </c>
-      <c r="B20" t="s">
-        <v>115</v>
-      </c>
-      <c r="C20">
-        <v>1</v>
-      </c>
-      <c r="D20" t="s">
-        <v>116</v>
-      </c>
-      <c r="E20" t="s">
-        <v>117</v>
-      </c>
-      <c r="F20" t="s">
-        <v>117</v>
-      </c>
-      <c r="H20" s="2">
-        <v>5262.66</v>
-      </c>
-      <c r="J20" t="s">
-        <v>118</v>
-      </c>
-      <c r="M20">
-        <f t="shared" ref="M20:M25" si="3">C20*H20</f>
-        <v>5262.66</v>
-      </c>
-    </row>
-    <row r="21" spans="1:13" x14ac:dyDescent="0.3">
-      <c r="A21">
-        <v>20</v>
-      </c>
-      <c r="B21" t="s">
-        <v>122</v>
-      </c>
-      <c r="C21">
-        <v>1</v>
-      </c>
-      <c r="D21" t="s">
-        <v>35</v>
-      </c>
-      <c r="E21" t="s">
-        <v>75</v>
-      </c>
-      <c r="F21" t="s">
-        <v>75</v>
-      </c>
-      <c r="H21" s="2">
-        <v>2985.2159999999999</v>
-      </c>
-      <c r="J21" t="s">
-        <v>123</v>
-      </c>
-      <c r="M21">
-        <f t="shared" si="3"/>
-        <v>2985.2159999999999</v>
-      </c>
-    </row>
-    <row r="22" spans="1:13" x14ac:dyDescent="0.3">
-      <c r="A22">
-        <v>21</v>
-      </c>
-      <c r="B22" t="s">
-        <v>124</v>
-      </c>
-      <c r="C22">
-        <v>1</v>
-      </c>
-      <c r="D22" t="s">
-        <v>90</v>
-      </c>
-      <c r="E22" t="s">
-        <v>125</v>
-      </c>
-      <c r="F22" t="s">
-        <v>125</v>
-      </c>
-      <c r="H22" s="2">
-        <v>1571.7</v>
-      </c>
-      <c r="J22" t="s">
-        <v>126</v>
-      </c>
-      <c r="M22">
-        <f t="shared" si="3"/>
-        <v>1571.7</v>
-      </c>
-    </row>
-    <row r="23" spans="1:13" x14ac:dyDescent="0.3">
-      <c r="A23">
-        <v>22</v>
-      </c>
-      <c r="B23" t="s">
-        <v>127</v>
-      </c>
-      <c r="C23">
-        <v>1</v>
-      </c>
-      <c r="D23" t="s">
-        <v>128</v>
-      </c>
-      <c r="E23" t="s">
-        <v>111</v>
-      </c>
-      <c r="F23" t="s">
-        <v>111</v>
-      </c>
-      <c r="H23" s="2">
-        <v>9873</v>
-      </c>
-      <c r="J23" t="s">
-        <v>129</v>
-      </c>
-      <c r="K23" t="s">
-        <v>130</v>
-      </c>
-      <c r="L23" t="s">
-        <v>131</v>
-      </c>
-      <c r="M23">
-        <f t="shared" si="3"/>
-        <v>9873</v>
-      </c>
-    </row>
-    <row r="24" spans="1:13" x14ac:dyDescent="0.3">
-      <c r="A24">
-        <v>23</v>
-      </c>
-      <c r="B24" t="s">
-        <v>145</v>
-      </c>
-      <c r="C24">
-        <v>1</v>
-      </c>
-      <c r="D24" t="s">
-        <v>146</v>
-      </c>
-      <c r="E24" t="s">
-        <v>147</v>
-      </c>
-      <c r="F24" t="s">
-        <v>148</v>
-      </c>
-      <c r="H24" s="2">
-        <v>6235.6944000000003</v>
-      </c>
-      <c r="J24" t="s">
-        <v>149</v>
-      </c>
-      <c r="M24">
-        <f t="shared" si="3"/>
-        <v>6235.6944000000003</v>
-      </c>
-    </row>
-    <row r="25" spans="1:13" x14ac:dyDescent="0.3">
-      <c r="A25">
-        <v>24</v>
-      </c>
-      <c r="B25" t="s">
-        <v>150</v>
-      </c>
-      <c r="C25">
-        <v>1</v>
-      </c>
-      <c r="D25" t="s">
-        <v>91</v>
-      </c>
-      <c r="E25" t="s">
-        <v>151</v>
-      </c>
-      <c r="F25" t="s">
-        <v>151</v>
-      </c>
-      <c r="H25" s="2">
-        <v>540.42899999999997</v>
-      </c>
-      <c r="J25" t="s">
-        <v>152</v>
-      </c>
-      <c r="K25" t="s">
-        <v>153</v>
-      </c>
-      <c r="L25" t="s">
-        <v>154</v>
-      </c>
-      <c r="M25">
-        <f t="shared" si="3"/>
-        <v>540.42899999999997</v>
-      </c>
-    </row>
-    <row r="26" spans="1:13" x14ac:dyDescent="0.3">
-      <c r="A26">
-        <v>25</v>
-      </c>
-      <c r="B26" t="s">
-        <v>155</v>
-      </c>
-      <c r="C26">
-        <v>1</v>
-      </c>
-      <c r="D26" t="s">
-        <v>156</v>
-      </c>
-      <c r="E26" t="s">
-        <v>157</v>
-      </c>
-      <c r="F26" t="s">
-        <v>157</v>
-      </c>
-      <c r="H26" s="2">
-        <v>447.899</v>
-      </c>
-      <c r="J26" t="s">
-        <v>152</v>
-      </c>
-      <c r="K26" t="s">
-        <v>158</v>
-      </c>
-      <c r="L26" t="s">
-        <v>159</v>
-      </c>
-      <c r="M26">
-        <f>C26*H26</f>
-        <v>447.899</v>
+        <f>C4*H4</f>
+        <v>3673.2150000000001</v>
       </c>
     </row>
   </sheetData>
@@ -1918,6 +1273,1044 @@
 </file>
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1954A817-8B83-4AEA-A467-593A05541A84}">
+  <dimension ref="A1:M31"/>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetData>
+    <row r="1" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A1" t="s">
+        <v>13</v>
+      </c>
+      <c r="B1" t="s">
+        <v>14</v>
+      </c>
+      <c r="C1" t="s">
+        <v>15</v>
+      </c>
+      <c r="D1" t="s">
+        <v>16</v>
+      </c>
+      <c r="E1" t="s">
+        <v>17</v>
+      </c>
+      <c r="F1" t="s">
+        <v>18</v>
+      </c>
+      <c r="G1" t="s">
+        <v>19</v>
+      </c>
+      <c r="H1" t="s">
+        <v>20</v>
+      </c>
+      <c r="I1" t="s">
+        <v>21</v>
+      </c>
+      <c r="J1" t="s">
+        <v>22</v>
+      </c>
+      <c r="K1" t="s">
+        <v>23</v>
+      </c>
+      <c r="L1" t="s">
+        <v>24</v>
+      </c>
+      <c r="M1" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="2" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A2">
+        <v>1</v>
+      </c>
+      <c r="B2" t="s">
+        <v>61</v>
+      </c>
+      <c r="C2">
+        <v>1</v>
+      </c>
+      <c r="D2">
+        <v>3</v>
+      </c>
+      <c r="E2">
+        <v>4</v>
+      </c>
+      <c r="F2">
+        <v>4</v>
+      </c>
+      <c r="H2" s="2">
+        <v>47324.537900000003</v>
+      </c>
+      <c r="J2" t="s">
+        <v>62</v>
+      </c>
+      <c r="K2" t="s">
+        <v>63</v>
+      </c>
+      <c r="L2" t="s">
+        <v>64</v>
+      </c>
+      <c r="M2">
+        <f t="shared" ref="M2:M7" si="0">C2*H2</f>
+        <v>47324.537900000003</v>
+      </c>
+    </row>
+    <row r="3" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A3">
+        <v>2</v>
+      </c>
+      <c r="B3" t="s">
+        <v>65</v>
+      </c>
+      <c r="C3">
+        <v>1</v>
+      </c>
+      <c r="D3" t="s">
+        <v>29</v>
+      </c>
+      <c r="E3" t="s">
+        <v>29</v>
+      </c>
+      <c r="F3" t="s">
+        <v>29</v>
+      </c>
+      <c r="G3">
+        <v>0</v>
+      </c>
+      <c r="H3" s="2">
+        <v>3843.9929000000002</v>
+      </c>
+      <c r="J3" t="s">
+        <v>66</v>
+      </c>
+      <c r="M3">
+        <f t="shared" si="0"/>
+        <v>3843.9929000000002</v>
+      </c>
+    </row>
+    <row r="4" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A4">
+        <v>3</v>
+      </c>
+      <c r="B4" t="s">
+        <v>67</v>
+      </c>
+      <c r="C4">
+        <v>1</v>
+      </c>
+      <c r="D4" t="s">
+        <v>68</v>
+      </c>
+      <c r="E4" t="s">
+        <v>69</v>
+      </c>
+      <c r="F4" t="s">
+        <v>70</v>
+      </c>
+      <c r="H4" s="2">
+        <v>3781.2494999999999</v>
+      </c>
+      <c r="J4" t="s">
+        <v>71</v>
+      </c>
+      <c r="K4" t="s">
+        <v>72</v>
+      </c>
+      <c r="L4" t="s">
+        <v>73</v>
+      </c>
+      <c r="M4">
+        <f t="shared" si="0"/>
+        <v>3781.2494999999999</v>
+      </c>
+    </row>
+    <row r="5" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A5">
+        <v>4</v>
+      </c>
+      <c r="B5" t="s">
+        <v>74</v>
+      </c>
+      <c r="C5">
+        <v>1</v>
+      </c>
+      <c r="D5" t="s">
+        <v>75</v>
+      </c>
+      <c r="E5" t="s">
+        <v>76</v>
+      </c>
+      <c r="F5" t="s">
+        <v>77</v>
+      </c>
+      <c r="H5" s="2">
+        <v>5282.1998000000003</v>
+      </c>
+      <c r="J5" t="s">
+        <v>78</v>
+      </c>
+      <c r="M5">
+        <f t="shared" si="0"/>
+        <v>5282.1998000000003</v>
+      </c>
+    </row>
+    <row r="6" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A6">
+        <v>5</v>
+      </c>
+      <c r="B6" t="s">
+        <v>79</v>
+      </c>
+      <c r="C6">
+        <v>1</v>
+      </c>
+      <c r="D6" t="s">
+        <v>80</v>
+      </c>
+      <c r="H6" s="2">
+        <v>2818.92</v>
+      </c>
+      <c r="J6" t="s">
+        <v>81</v>
+      </c>
+      <c r="K6" t="s">
+        <v>82</v>
+      </c>
+      <c r="L6" t="s">
+        <v>83</v>
+      </c>
+      <c r="M6">
+        <f t="shared" si="0"/>
+        <v>2818.92</v>
+      </c>
+    </row>
+    <row r="7" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A7">
+        <v>6</v>
+      </c>
+      <c r="B7" t="s">
+        <v>84</v>
+      </c>
+      <c r="C7">
+        <v>1</v>
+      </c>
+      <c r="D7" t="s">
+        <v>85</v>
+      </c>
+      <c r="H7" s="2">
+        <v>951.5376</v>
+      </c>
+      <c r="J7" t="s">
+        <v>86</v>
+      </c>
+      <c r="K7" t="s">
+        <v>87</v>
+      </c>
+      <c r="L7" t="s">
+        <v>88</v>
+      </c>
+      <c r="M7">
+        <f t="shared" si="0"/>
+        <v>951.5376</v>
+      </c>
+    </row>
+    <row r="8" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A8">
+        <v>7</v>
+      </c>
+      <c r="B8" t="s">
+        <v>89</v>
+      </c>
+      <c r="C8">
+        <v>1</v>
+      </c>
+      <c r="D8" t="s">
+        <v>90</v>
+      </c>
+      <c r="E8" t="s">
+        <v>91</v>
+      </c>
+      <c r="F8" t="s">
+        <v>91</v>
+      </c>
+      <c r="H8" s="2">
+        <v>407.93220000000002</v>
+      </c>
+      <c r="J8" t="s">
+        <v>92</v>
+      </c>
+      <c r="K8" t="s">
+        <v>93</v>
+      </c>
+      <c r="L8" t="s">
+        <v>94</v>
+      </c>
+      <c r="M8">
+        <f t="shared" ref="M8:M13" si="1">C8*H8</f>
+        <v>407.93220000000002</v>
+      </c>
+    </row>
+    <row r="9" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A9">
+        <v>8</v>
+      </c>
+      <c r="B9" t="s">
+        <v>95</v>
+      </c>
+      <c r="C9">
+        <v>1</v>
+      </c>
+      <c r="D9" t="s">
+        <v>96</v>
+      </c>
+      <c r="E9" t="s">
+        <v>77</v>
+      </c>
+      <c r="F9">
+        <v>6</v>
+      </c>
+      <c r="H9" s="2">
+        <v>70702.5</v>
+      </c>
+      <c r="J9" t="s">
+        <v>97</v>
+      </c>
+      <c r="K9" t="s">
+        <v>98</v>
+      </c>
+      <c r="L9" t="s">
+        <v>99</v>
+      </c>
+      <c r="M9">
+        <f t="shared" si="1"/>
+        <v>70702.5</v>
+      </c>
+    </row>
+    <row r="10" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A10">
+        <v>9</v>
+      </c>
+      <c r="B10" t="s">
+        <v>100</v>
+      </c>
+      <c r="C10">
+        <v>1</v>
+      </c>
+      <c r="D10" t="s">
+        <v>101</v>
+      </c>
+      <c r="E10" t="s">
+        <v>75</v>
+      </c>
+      <c r="F10" t="s">
+        <v>75</v>
+      </c>
+      <c r="H10" s="2">
+        <v>4370.9639999999999</v>
+      </c>
+      <c r="J10" t="s">
+        <v>102</v>
+      </c>
+      <c r="K10" t="s">
+        <v>103</v>
+      </c>
+      <c r="L10" t="s">
+        <v>104</v>
+      </c>
+      <c r="M10">
+        <f t="shared" si="1"/>
+        <v>4370.9639999999999</v>
+      </c>
+    </row>
+    <row r="11" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A11">
+        <v>10</v>
+      </c>
+      <c r="B11" t="s">
+        <v>105</v>
+      </c>
+      <c r="C11">
+        <v>1</v>
+      </c>
+      <c r="D11" t="s">
+        <v>29</v>
+      </c>
+      <c r="E11" t="s">
+        <v>106</v>
+      </c>
+      <c r="F11" t="s">
+        <v>107</v>
+      </c>
+      <c r="H11" s="2">
+        <v>25450</v>
+      </c>
+      <c r="J11" t="s">
+        <v>108</v>
+      </c>
+      <c r="L11" t="s">
+        <v>109</v>
+      </c>
+      <c r="M11">
+        <f t="shared" si="1"/>
+        <v>25450</v>
+      </c>
+    </row>
+    <row r="12" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A12">
+        <v>11</v>
+      </c>
+      <c r="B12" t="s">
+        <v>110</v>
+      </c>
+      <c r="C12">
+        <v>1</v>
+      </c>
+      <c r="D12" t="s">
+        <v>111</v>
+      </c>
+      <c r="E12" t="s">
+        <v>76</v>
+      </c>
+      <c r="F12" t="s">
+        <v>76</v>
+      </c>
+      <c r="H12" s="2">
+        <v>6624.7093000000004</v>
+      </c>
+      <c r="J12" t="s">
+        <v>112</v>
+      </c>
+      <c r="K12" t="s">
+        <v>113</v>
+      </c>
+      <c r="L12" t="s">
+        <v>114</v>
+      </c>
+      <c r="M12">
+        <f t="shared" si="1"/>
+        <v>6624.7093000000004</v>
+      </c>
+    </row>
+    <row r="13" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A13">
+        <v>12</v>
+      </c>
+      <c r="B13" t="s">
+        <v>115</v>
+      </c>
+      <c r="C13">
+        <v>1</v>
+      </c>
+      <c r="D13" t="s">
+        <v>116</v>
+      </c>
+      <c r="E13" t="s">
+        <v>117</v>
+      </c>
+      <c r="F13" t="s">
+        <v>117</v>
+      </c>
+      <c r="H13" s="2">
+        <v>5262.66</v>
+      </c>
+      <c r="J13" t="s">
+        <v>118</v>
+      </c>
+      <c r="M13">
+        <f t="shared" si="1"/>
+        <v>5262.66</v>
+      </c>
+    </row>
+    <row r="14" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A14">
+        <v>13</v>
+      </c>
+      <c r="B14" t="s">
+        <v>122</v>
+      </c>
+      <c r="C14">
+        <v>1</v>
+      </c>
+      <c r="D14" t="s">
+        <v>35</v>
+      </c>
+      <c r="E14" t="s">
+        <v>75</v>
+      </c>
+      <c r="F14" t="s">
+        <v>75</v>
+      </c>
+      <c r="H14" s="2">
+        <v>2985.2159999999999</v>
+      </c>
+      <c r="J14" t="s">
+        <v>123</v>
+      </c>
+      <c r="M14">
+        <f t="shared" ref="M14:M19" si="2">C14*H14</f>
+        <v>2985.2159999999999</v>
+      </c>
+    </row>
+    <row r="15" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A15">
+        <v>14</v>
+      </c>
+      <c r="B15" t="s">
+        <v>124</v>
+      </c>
+      <c r="C15">
+        <v>1</v>
+      </c>
+      <c r="D15" t="s">
+        <v>90</v>
+      </c>
+      <c r="E15" t="s">
+        <v>125</v>
+      </c>
+      <c r="F15" t="s">
+        <v>125</v>
+      </c>
+      <c r="H15" s="2">
+        <v>1571.7</v>
+      </c>
+      <c r="J15" t="s">
+        <v>126</v>
+      </c>
+      <c r="M15">
+        <f t="shared" si="2"/>
+        <v>1571.7</v>
+      </c>
+    </row>
+    <row r="16" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A16">
+        <v>15</v>
+      </c>
+      <c r="B16" t="s">
+        <v>127</v>
+      </c>
+      <c r="C16">
+        <v>1</v>
+      </c>
+      <c r="D16" t="s">
+        <v>128</v>
+      </c>
+      <c r="E16" t="s">
+        <v>111</v>
+      </c>
+      <c r="F16" t="s">
+        <v>111</v>
+      </c>
+      <c r="H16" s="2">
+        <v>9873</v>
+      </c>
+      <c r="J16" t="s">
+        <v>129</v>
+      </c>
+      <c r="K16" t="s">
+        <v>130</v>
+      </c>
+      <c r="L16" t="s">
+        <v>131</v>
+      </c>
+      <c r="M16">
+        <f t="shared" si="2"/>
+        <v>9873</v>
+      </c>
+    </row>
+    <row r="17" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A17">
+        <v>16</v>
+      </c>
+      <c r="B17" t="s">
+        <v>132</v>
+      </c>
+      <c r="D17">
+        <v>15</v>
+      </c>
+      <c r="E17" t="s">
+        <v>133</v>
+      </c>
+      <c r="F17" t="s">
+        <v>134</v>
+      </c>
+      <c r="H17" s="2">
+        <v>0</v>
+      </c>
+      <c r="J17" t="s">
+        <v>135</v>
+      </c>
+      <c r="K17" t="s">
+        <v>136</v>
+      </c>
+      <c r="L17" t="s">
+        <v>137</v>
+      </c>
+      <c r="M17">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="18" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A18">
+        <v>17</v>
+      </c>
+      <c r="B18" t="s">
+        <v>138</v>
+      </c>
+      <c r="C18">
+        <v>1</v>
+      </c>
+      <c r="H18" s="2">
+        <v>0</v>
+      </c>
+      <c r="J18" t="s">
+        <v>139</v>
+      </c>
+      <c r="M18">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="19" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A19">
+        <v>18</v>
+      </c>
+      <c r="B19" t="s">
+        <v>140</v>
+      </c>
+      <c r="C19">
+        <v>1</v>
+      </c>
+      <c r="D19">
+        <v>15</v>
+      </c>
+      <c r="E19" t="s">
+        <v>133</v>
+      </c>
+      <c r="F19" t="s">
+        <v>134</v>
+      </c>
+      <c r="H19" s="2">
+        <v>0</v>
+      </c>
+      <c r="J19" t="s">
+        <v>141</v>
+      </c>
+      <c r="K19" t="s">
+        <v>142</v>
+      </c>
+      <c r="L19" t="s">
+        <v>143</v>
+      </c>
+      <c r="M19">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="20" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A20">
+        <v>19</v>
+      </c>
+      <c r="B20" t="s">
+        <v>115</v>
+      </c>
+      <c r="C20">
+        <v>1</v>
+      </c>
+      <c r="D20" t="s">
+        <v>116</v>
+      </c>
+      <c r="E20" t="s">
+        <v>117</v>
+      </c>
+      <c r="F20" t="s">
+        <v>117</v>
+      </c>
+      <c r="H20" s="2">
+        <v>5262.66</v>
+      </c>
+      <c r="J20" t="s">
+        <v>118</v>
+      </c>
+      <c r="M20">
+        <f t="shared" ref="M20:M25" si="3">C20*H20</f>
+        <v>5262.66</v>
+      </c>
+    </row>
+    <row r="21" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A21">
+        <v>20</v>
+      </c>
+      <c r="B21" t="s">
+        <v>122</v>
+      </c>
+      <c r="C21">
+        <v>1</v>
+      </c>
+      <c r="D21" t="s">
+        <v>35</v>
+      </c>
+      <c r="E21" t="s">
+        <v>75</v>
+      </c>
+      <c r="F21" t="s">
+        <v>75</v>
+      </c>
+      <c r="H21" s="2">
+        <v>2985.2159999999999</v>
+      </c>
+      <c r="J21" t="s">
+        <v>123</v>
+      </c>
+      <c r="M21">
+        <f t="shared" si="3"/>
+        <v>2985.2159999999999</v>
+      </c>
+    </row>
+    <row r="22" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A22">
+        <v>21</v>
+      </c>
+      <c r="B22" t="s">
+        <v>124</v>
+      </c>
+      <c r="C22">
+        <v>1</v>
+      </c>
+      <c r="D22" t="s">
+        <v>90</v>
+      </c>
+      <c r="E22" t="s">
+        <v>125</v>
+      </c>
+      <c r="F22" t="s">
+        <v>125</v>
+      </c>
+      <c r="H22" s="2">
+        <v>1571.7</v>
+      </c>
+      <c r="J22" t="s">
+        <v>126</v>
+      </c>
+      <c r="M22">
+        <f t="shared" si="3"/>
+        <v>1571.7</v>
+      </c>
+    </row>
+    <row r="23" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A23">
+        <v>22</v>
+      </c>
+      <c r="B23" t="s">
+        <v>127</v>
+      </c>
+      <c r="C23">
+        <v>1</v>
+      </c>
+      <c r="D23" t="s">
+        <v>128</v>
+      </c>
+      <c r="E23" t="s">
+        <v>111</v>
+      </c>
+      <c r="F23" t="s">
+        <v>111</v>
+      </c>
+      <c r="H23" s="2">
+        <v>9873</v>
+      </c>
+      <c r="J23" t="s">
+        <v>129</v>
+      </c>
+      <c r="K23" t="s">
+        <v>130</v>
+      </c>
+      <c r="L23" t="s">
+        <v>131</v>
+      </c>
+      <c r="M23">
+        <f t="shared" si="3"/>
+        <v>9873</v>
+      </c>
+    </row>
+    <row r="24" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A24">
+        <v>23</v>
+      </c>
+      <c r="B24" t="s">
+        <v>145</v>
+      </c>
+      <c r="C24">
+        <v>1</v>
+      </c>
+      <c r="D24" t="s">
+        <v>146</v>
+      </c>
+      <c r="E24" t="s">
+        <v>147</v>
+      </c>
+      <c r="F24" t="s">
+        <v>148</v>
+      </c>
+      <c r="H24" s="2">
+        <v>6235.6944000000003</v>
+      </c>
+      <c r="J24" t="s">
+        <v>149</v>
+      </c>
+      <c r="M24">
+        <f t="shared" si="3"/>
+        <v>6235.6944000000003</v>
+      </c>
+    </row>
+    <row r="25" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A25">
+        <v>24</v>
+      </c>
+      <c r="B25" t="s">
+        <v>150</v>
+      </c>
+      <c r="C25">
+        <v>1</v>
+      </c>
+      <c r="D25" t="s">
+        <v>91</v>
+      </c>
+      <c r="E25" t="s">
+        <v>151</v>
+      </c>
+      <c r="F25" t="s">
+        <v>151</v>
+      </c>
+      <c r="H25" s="2">
+        <v>540.42899999999997</v>
+      </c>
+      <c r="J25" t="s">
+        <v>152</v>
+      </c>
+      <c r="K25" t="s">
+        <v>153</v>
+      </c>
+      <c r="L25" t="s">
+        <v>154</v>
+      </c>
+      <c r="M25">
+        <f t="shared" si="3"/>
+        <v>540.42899999999997</v>
+      </c>
+    </row>
+    <row r="26" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A26">
+        <v>25</v>
+      </c>
+      <c r="B26" t="s">
+        <v>155</v>
+      </c>
+      <c r="C26">
+        <v>1</v>
+      </c>
+      <c r="D26" t="s">
+        <v>156</v>
+      </c>
+      <c r="E26" t="s">
+        <v>157</v>
+      </c>
+      <c r="F26" t="s">
+        <v>157</v>
+      </c>
+      <c r="H26" s="2">
+        <v>447.899</v>
+      </c>
+      <c r="J26" t="s">
+        <v>152</v>
+      </c>
+      <c r="K26" t="s">
+        <v>158</v>
+      </c>
+      <c r="L26" t="s">
+        <v>159</v>
+      </c>
+      <c r="M26">
+        <f t="shared" ref="M26:M31" si="4">C26*H26</f>
+        <v>447.899</v>
+      </c>
+    </row>
+    <row r="27" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A27">
+        <v>26</v>
+      </c>
+      <c r="B27" t="s">
+        <v>160</v>
+      </c>
+      <c r="C27">
+        <v>1</v>
+      </c>
+      <c r="D27" t="s">
+        <v>90</v>
+      </c>
+      <c r="E27" t="s">
+        <v>161</v>
+      </c>
+      <c r="F27" t="s">
+        <v>162</v>
+      </c>
+      <c r="H27" s="2">
+        <v>851.87149999999997</v>
+      </c>
+      <c r="J27" t="s">
+        <v>152</v>
+      </c>
+      <c r="K27" t="s">
+        <v>163</v>
+      </c>
+      <c r="L27" t="s">
+        <v>164</v>
+      </c>
+      <c r="M27">
+        <f t="shared" si="4"/>
+        <v>851.87149999999997</v>
+      </c>
+    </row>
+    <row r="28" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A28">
+        <v>27</v>
+      </c>
+      <c r="B28" t="s">
+        <v>165</v>
+      </c>
+      <c r="C28">
+        <v>1</v>
+      </c>
+      <c r="D28" t="s">
+        <v>85</v>
+      </c>
+      <c r="H28" s="2">
+        <v>951.5376</v>
+      </c>
+      <c r="J28" t="s">
+        <v>92</v>
+      </c>
+      <c r="K28" t="s">
+        <v>166</v>
+      </c>
+      <c r="L28" t="s">
+        <v>167</v>
+      </c>
+      <c r="M28">
+        <f t="shared" si="4"/>
+        <v>951.5376</v>
+      </c>
+    </row>
+    <row r="29" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A29">
+        <v>28</v>
+      </c>
+      <c r="B29" t="s">
+        <v>168</v>
+      </c>
+      <c r="C29">
+        <v>1</v>
+      </c>
+      <c r="D29" t="s">
+        <v>90</v>
+      </c>
+      <c r="E29" t="s">
+        <v>91</v>
+      </c>
+      <c r="F29" t="s">
+        <v>91</v>
+      </c>
+      <c r="H29" s="2">
+        <v>407.93220000000002</v>
+      </c>
+      <c r="J29" t="s">
+        <v>81</v>
+      </c>
+      <c r="K29" t="s">
+        <v>169</v>
+      </c>
+      <c r="L29" t="s">
+        <v>170</v>
+      </c>
+      <c r="M29">
+        <f t="shared" si="4"/>
+        <v>407.93220000000002</v>
+      </c>
+    </row>
+    <row r="30" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A30">
+        <v>29</v>
+      </c>
+      <c r="B30" t="s">
+        <v>65</v>
+      </c>
+      <c r="C30">
+        <v>1</v>
+      </c>
+      <c r="D30" t="s">
+        <v>29</v>
+      </c>
+      <c r="E30" t="s">
+        <v>29</v>
+      </c>
+      <c r="F30" t="s">
+        <v>29</v>
+      </c>
+      <c r="G30">
+        <v>0</v>
+      </c>
+      <c r="H30" s="2">
+        <v>3843.9929000000002</v>
+      </c>
+      <c r="J30" t="s">
+        <v>66</v>
+      </c>
+      <c r="M30">
+        <f t="shared" si="4"/>
+        <v>3843.9929000000002</v>
+      </c>
+    </row>
+    <row r="31" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A31">
+        <v>30</v>
+      </c>
+      <c r="B31" t="s">
+        <v>171</v>
+      </c>
+      <c r="C31">
+        <v>1</v>
+      </c>
+      <c r="D31" t="s">
+        <v>172</v>
+      </c>
+      <c r="E31" t="s">
+        <v>173</v>
+      </c>
+      <c r="F31" t="s">
+        <v>174</v>
+      </c>
+      <c r="G31">
+        <v>0</v>
+      </c>
+      <c r="H31" s="2">
+        <v>9037.0722000000005</v>
+      </c>
+      <c r="J31" t="s">
+        <v>175</v>
+      </c>
+      <c r="M31">
+        <f t="shared" si="4"/>
+        <v>9037.0722000000005</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5D53E6AF-1635-462B-BD5B-E2C2FFDBFB8E}">
   <dimension ref="A1:M10"/>
   <sheetViews>

</xml_diff>